<commit_message>
Added in data extraction file
</commit_message>
<xml_diff>
--- a/_output/2. Extension - Oct 2024/Results.xlsx
+++ b/_output/2. Extension - Oct 2024/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hons2024\Desktop\Extension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Research Project\OFA-research-project\OFA-research-project\_output\2. Extension - Oct 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05037B5-3B22-4D22-AFC4-52157F6EC033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3C16E8-91D2-4B79-846F-941B0D45B1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="180" windowWidth="19545" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t>Price Series</t>
   </si>
@@ -184,9 +184,6 @@
     <t>sig_TFI</t>
   </si>
   <si>
-    <t>alpha</t>
-  </si>
-  <si>
     <t>1 sec</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>847.214858</t>
   </si>
   <si>
-    <t>0.2520625310</t>
-  </si>
-  <si>
     <t>100.00000</t>
   </si>
   <si>
@@ -214,12 +208,6 @@
     <t>238.48038</t>
   </si>
   <si>
-    <t>0.1205739</t>
-  </si>
-  <si>
-    <t>alpha1</t>
-  </si>
-  <si>
     <t>10 secs</t>
   </si>
   <si>
@@ -232,9 +220,6 @@
     <t>264.997057</t>
   </si>
   <si>
-    <t>0.2085641731</t>
-  </si>
-  <si>
     <t>0.3420663</t>
   </si>
   <si>
@@ -244,12 +229,6 @@
     <t>154.02427</t>
   </si>
   <si>
-    <t>0.1197789</t>
-  </si>
-  <si>
-    <t>alpha2</t>
-  </si>
-  <si>
     <t>-3.8186312</t>
   </si>
   <si>
@@ -259,9 +238,6 @@
     <t>65.462470</t>
   </si>
   <si>
-    <t>0.0875946530</t>
-  </si>
-  <si>
     <t>1.5443112</t>
   </si>
   <si>
@@ -271,12 +247,6 @@
     <t>91.44317</t>
   </si>
   <si>
-    <t>0.1621839</t>
-  </si>
-  <si>
-    <t>alpha3</t>
-  </si>
-  <si>
     <t>5 mins</t>
   </si>
   <si>
@@ -289,9 +259,6 @@
     <t>8.691963</t>
   </si>
   <si>
-    <t>0.0083939551</t>
-  </si>
-  <si>
     <t>7.3748424</t>
   </si>
   <si>
@@ -301,12 +268,6 @@
     <t>48.30567</t>
   </si>
   <si>
-    <t>0.2073165</t>
-  </si>
-  <si>
-    <t>alpha4</t>
-  </si>
-  <si>
     <t>10 mins</t>
   </si>
   <si>
@@ -319,9 +280,6 @@
     <t>1.192017</t>
   </si>
   <si>
-    <t>0.0003184157</t>
-  </si>
-  <si>
     <t>76.66820</t>
   </si>
   <si>
@@ -334,12 +292,6 @@
     <t>35.37613</t>
   </si>
   <si>
-    <t>0.2191153</t>
-  </si>
-  <si>
-    <t>alpha5</t>
-  </si>
-  <si>
     <t>1 hour</t>
   </si>
   <si>
@@ -352,9 +304,6 @@
     <t>-2.685818</t>
   </si>
   <si>
-    <t>0.0096411232</t>
-  </si>
-  <si>
     <t>99.26028</t>
   </si>
   <si>
@@ -365,9 +314,6 @@
   </si>
   <si>
     <t>16.75711</t>
-  </si>
-  <si>
-    <t>0.2748096</t>
   </si>
   <si>
     <t>kable(ofi_stationarity_urca, digits = 5,</t>
@@ -431,6 +377,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,7 +439,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -500,6 +449,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -572,6 +527,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1479,7 @@
       <c r="A46" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="16" t="s">
@@ -1530,218 +1488,200 @@
       <c r="D46" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="20">
+        <v>0.25206253099999998</v>
+      </c>
+      <c r="F46" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="G46" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G46" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="I46" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="I46" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="J46" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K46" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="L46" s="16">
+      <c r="J46" s="20">
+        <v>0.1205739</v>
+      </c>
+      <c r="K46" s="16">
         <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="E47" s="20">
+        <v>0.2085641731</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="I47" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="J47" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="K47" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="L47" s="16">
+      <c r="J47" s="20">
+        <v>0.11977889999999999</v>
+      </c>
+      <c r="K47" s="16">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="20">
+        <v>8.7594652999999995E-2</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" s="20">
+        <v>0.16218389999999999</v>
+      </c>
+      <c r="K48" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="16" t="s">
+      <c r="B49" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="C49" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="E49" s="20">
+        <v>8.3939550999999994E-3</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G48" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H48" s="16" t="s">
+      <c r="H49" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="I48" s="16" t="s">
+      <c r="I49" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J48" s="16" t="s">
+      <c r="J49" s="20">
+        <v>0.20731649999999999</v>
+      </c>
+      <c r="K49" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="K48" s="16" t="s">
+      <c r="B50" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="L48" s="16">
+      <c r="C50" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="20">
+        <v>3.1841569999999997E-4</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J50" s="20">
+        <v>0.21911530000000001</v>
+      </c>
+      <c r="K50" s="16">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H49" s="16" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="B51" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J49" s="16" t="s">
+      <c r="C51" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K49" s="16" t="s">
+      <c r="D51" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L49" s="16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="E51" s="20">
+        <v>9.6411232000000006E-3</v>
+      </c>
+      <c r="F51" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="G51" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="H51" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="I51" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E50" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="I50" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J50" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="K50" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="L50" s="16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="I51" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="J51" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="K51" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="L51" s="16">
+      <c r="J51" s="20">
+        <v>0.27480959999999999</v>
+      </c>
+      <c r="K51" s="16">
         <v>100</v>
       </c>
     </row>
@@ -1763,12 +1703,12 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1779,7 +1719,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1797,47 +1737,47 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1848,7 +1788,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -1866,32 +1806,32 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trade arrival stats added
</commit_message>
<xml_diff>
--- a/_output/2. Extension - Oct 2024/Results.xlsx
+++ b/_output/2. Extension - Oct 2024/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Research Project\OFA-research-project\OFA-research-project\_output\2. Extension - Oct 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\OFA-research-project\_output\2. Extension - Oct 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3C16E8-91D2-4B79-846F-941B0D45B1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4DF311-DE3E-4A28-978B-A9D270781559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="180" windowWidth="19545" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="118">
   <si>
     <t>Price Series</t>
   </si>
@@ -371,6 +371,15 @@
   </si>
   <si>
     <t>|1 hour   |     -18.02481|       -3.43|        0.06282|        0.739|</t>
+  </si>
+  <si>
+    <t>Arrival Stats: Trades XBTUSD - trade count per minute (trade frequency)</t>
+  </si>
+  <si>
+    <t>Arrival Stats: Trades XBTUSD - trade volume per minute (trade intensity)</t>
+  </si>
+  <si>
+    <t>Arrival Stats: Trades SPY.N ---- S&amp;P 500 ETF Trust - trade volume per minute (trade intensity)</t>
   </si>
 </sst>
 </file>
@@ -378,7 +387,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -528,7 +537,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,6 +558,143 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>162990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F666B430-F58F-486B-B918-969F0B80BADD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38101" y="9791700"/>
+          <a:ext cx="4162425" cy="505890"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>800099</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3796E224-0655-9FF0-B575-D4D9BD79093E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11591925"/>
+          <a:ext cx="4133849" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>45878</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86A82A42-4D36-1B95-6AAC-2B0A73F9E1BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="10677525"/>
+          <a:ext cx="4152900" cy="585628"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1101,81 +1247,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1183,7 +1329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -1227,7 +1373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
@@ -1271,7 +1417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
@@ -1315,95 +1461,95 @@
         <v>8708</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I19" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>40</v>
       </c>
@@ -1439,7 +1585,7 @@
       </c>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>41</v>
       </c>
@@ -1475,7 +1621,7 @@
       </c>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
         <v>52</v>
       </c>
@@ -1510,7 +1656,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
         <v>60</v>
       </c>
@@ -1545,7 +1691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
         <v>19</v>
       </c>
@@ -1580,7 +1726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
         <v>73</v>
       </c>
@@ -1615,7 +1761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
         <v>80</v>
       </c>
@@ -1650,7 +1796,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
         <v>88</v>
       </c>
@@ -1683,11 +1829,27 @@
       </c>
       <c r="K51" s="16">
         <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1699,137 +1861,137 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="18"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="18"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>114</v>
       </c>

</xml_diff>